<commit_message>
not important. Just tried to comment what I've known with the syntax
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -518,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
add parse.js and cell.js
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25823"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="100" windowWidth="23720" windowHeight="13920" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="96" windowWidth="23724" windowHeight="13920"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
     <sheet name="工作表2" sheetId="2" r:id="rId2"/>
     <sheet name="工作表3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -82,13 +82,13 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -97,7 +97,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -105,14 +105,14 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -120,7 +120,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -222,47 +222,47 @@
     </xf>
   </cellXfs>
   <cellStyles count="41">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="超連結" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="39" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -566,27 +566,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -594,7 +595,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -602,22 +603,22 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>10</v>
       </c>
@@ -638,20 +639,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" activeCellId="1" sqref="F18 G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="8.83203125" style="1"/>
+    <col min="3" max="3" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" style="6" customWidth="1"/>
+    <col min="5" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -665,7 +666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -679,7 +680,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -693,7 +694,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -707,7 +708,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -721,7 +722,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
@@ -735,7 +736,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -749,7 +750,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -763,7 +764,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -777,31 +778,31 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="5"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -825,7 +826,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>